<commit_message>
Adding TC006 which is as same as TC003
</commit_message>
<xml_diff>
--- a/Gmail/testdata/testdata.xlsx
+++ b/Gmail/testdata/testdata.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19380" windowHeight="6015" activeTab="2"/>
   </bookViews>
@@ -11,10 +11,9 @@
     <sheet name="TC002" sheetId="2" r:id="rId2"/>
     <sheet name="TC003" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <oleSize ref="A1:S18"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -66,8 +65,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -183,7 +182,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -218,7 +217,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -395,29 +394,30 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" customWidth="1"/>
+    <col min="5" max="6" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -438,7 +438,7 @@
       </c>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -459,7 +459,7 @@
       </c>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -474,16 +474,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -503,7 +503,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -529,16 +529,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -558,7 +561,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -578,7 +581,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -598,7 +601,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>

</xml_diff>